<commit_message>
Small adjustments to track likelihood of multiple variables
</commit_message>
<xml_diff>
--- a/PWP case/PWP_proxy_data_seasonal.xlsx
+++ b/PWP case/PWP_proxy_data_seasonal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Side projects\Bayesian temperature models\Seasonal DA\PWP case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwi213\Dropbox\Research\Side projects\Bayesian temperature models\Seasonal DA\SeasonalDA_script\PWP case\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE44846-79EB-47A8-B92C-CE20FC64FED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF0D337-2907-4614-AF05-84BE3C457C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C934B07A-2A76-40CE-8F43-0B267CC5ABE9}"/>
+    <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{C934B07A-2A76-40CE-8F43-0B267CC5ABE9}"/>
   </bookViews>
   <sheets>
     <sheet name="PWP_proxy_data_seasonal" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
   <si>
     <t>season_score</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>season</t>
+  </si>
+  <si>
+    <t>SD_ext</t>
   </si>
 </sst>
 </file>
@@ -1035,14 +1038,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E801C9-A2C4-48CE-B790-E5AB869422C6}">
-  <dimension ref="A1:AA26"/>
+  <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2:AA26"/>
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1143,8 +1148,8 @@
         <v>1.3542432120000001</v>
       </c>
       <c r="E2" s="1">
-        <f>(D2-C2)/2/TINV(0.05,$X2)*SQRT($X2)</f>
-        <v>0.28784575458710332</v>
+        <f>SQRT(((D2-C2)/2/TINV(0.05,$X2)*SQRT($X2))^2+E$32^2)</f>
+        <v>0.29840138183728471</v>
       </c>
       <c r="F2">
         <v>2.2901687119999998</v>
@@ -1156,8 +1161,8 @@
         <v>2.4833317400000001</v>
       </c>
       <c r="I2" s="1">
-        <f>(H2-G2)/2/TINV(0.05,$X2)*SQRT($X2)</f>
-        <v>0.18127781887572902</v>
+        <f>SQRT(((H2-G2)/2/TINV(0.05,$X2)*SQRT($X2))^2+I$32^2)</f>
+        <v>0.21973022985518148</v>
       </c>
       <c r="J2">
         <v>0.61008185500000001</v>
@@ -1232,8 +1237,8 @@
         <v>1.337010987</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E26" si="0">(D3-C3)/2/TINV(0.05,$X3)*SQRT($X3)</f>
-        <v>0.4861700215071284</v>
+        <f t="shared" ref="E3:E26" si="0">SQRT(((D3-C3)/2/TINV(0.05,$X3)*SQRT($X3))^2+E$32^2)</f>
+        <v>0.49249314316122594</v>
       </c>
       <c r="F3">
         <v>2.2391172639999999</v>
@@ -1245,8 +1250,8 @@
         <v>2.3407201450000001</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I26" si="1">(H3-G3)/2/TINV(0.05,$X3)*SQRT($X3)</f>
-        <v>0.26900927775416006</v>
+        <f t="shared" ref="I3:I26" si="1">SQRT(((H3-G3)/2/TINV(0.05,$X3)*SQRT($X3))^2+I$32^2)</f>
+        <v>0.2962865467983386</v>
       </c>
       <c r="J3">
         <v>0.63734738199999996</v>
@@ -1322,7 +1327,7 @@
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>0.22287408310585841</v>
+        <v>0.23634945138260668</v>
       </c>
       <c r="F4">
         <v>1.6305820609999999</v>
@@ -1335,7 +1340,7 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" si="1"/>
-        <v>0.47538930967544391</v>
+        <v>0.49133972162808531</v>
       </c>
       <c r="J4">
         <v>0.66107721500000005</v>
@@ -1411,7 +1416,7 @@
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>0.12889365099853098</v>
+        <v>0.15100258115778417</v>
       </c>
       <c r="F5">
         <v>2.4239481340000002</v>
@@ -1424,7 +1429,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="1"/>
-        <v>0.22062650823446575</v>
+        <v>0.25317144868962227</v>
       </c>
       <c r="J5">
         <v>0.64756084199999997</v>
@@ -1500,7 +1505,7 @@
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>3.0389549180058713E-2</v>
+        <v>8.4331079371423312E-2</v>
       </c>
       <c r="F6">
         <v>1.8275589590000001</v>
@@ -1513,7 +1518,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="1"/>
-        <v>2.8475386871551316E-2</v>
+        <v>0.12739926983053626</v>
       </c>
       <c r="J6">
         <v>0.65640470200000001</v>
@@ -1589,7 +1594,7 @@
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>0.16787198666038852</v>
+        <v>0.18538934746604982</v>
       </c>
       <c r="F7">
         <v>2.294876377</v>
@@ -1602,7 +1607,7 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="1"/>
-        <v>0.15776721901759164</v>
+        <v>0.20077405632305684</v>
       </c>
       <c r="J7">
         <v>0.64444523099999995</v>
@@ -1678,7 +1683,7 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>0.21219946119656249</v>
+        <v>0.22631132888278818</v>
       </c>
       <c r="F8">
         <v>1.4628680080000001</v>
@@ -1691,7 +1696,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>9.0056009930024578E-2</v>
+        <v>0.15339429983016303</v>
       </c>
       <c r="J8">
         <v>0.60801703200000001</v>
@@ -1767,7 +1772,7 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>3.4003537067374946E-2</v>
+        <v>8.5699747850705096E-2</v>
       </c>
       <c r="F9">
         <v>2.6198237780000002</v>
@@ -1780,7 +1785,7 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="1"/>
-        <v>4.3948558470292887E-2</v>
+        <v>0.13172396170585676</v>
       </c>
       <c r="J9">
         <v>0.63446967799999998</v>
@@ -1856,7 +1861,7 @@
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>9.1827737193274042E-2</v>
+        <v>0.1209154231957987</v>
       </c>
       <c r="F10">
         <v>0.57931777500000003</v>
@@ -1869,7 +1874,7 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>9.0718262397611632E-2</v>
+        <v>0.15378403502415713</v>
       </c>
       <c r="J10">
         <v>0.64204430700000004</v>
@@ -1945,7 +1950,7 @@
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
-        <v>0.26972158885442227</v>
+        <v>0.28095896807672127</v>
       </c>
       <c r="F11">
         <v>0.86542770899999999</v>
@@ -1958,7 +1963,7 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="1"/>
-        <v>0.16812215902964991</v>
+        <v>0.20900905878133647</v>
       </c>
       <c r="J11">
         <v>0.64983402300000004</v>
@@ -2034,7 +2039,7 @@
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>0.54785918479335649</v>
+        <v>0.55347799650123697</v>
       </c>
       <c r="F12">
         <v>0.46009582500000001</v>
@@ -2047,7 +2052,7 @@
       </c>
       <c r="I12" s="1">
         <f t="shared" si="1"/>
-        <v>0.16841991315434959</v>
+        <v>0.20924864024119233</v>
       </c>
       <c r="J12">
         <v>0.60813092800000002</v>
@@ -2123,7 +2128,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
-        <v>0.57550482499070732</v>
+        <v>0.5808562729592982</v>
       </c>
       <c r="F13">
         <v>0.89598664299999997</v>
@@ -2136,7 +2141,7 @@
       </c>
       <c r="I13" s="1">
         <f t="shared" si="1"/>
-        <v>0.15084152166121109</v>
+        <v>0.1953788395731198</v>
       </c>
       <c r="J13">
         <v>0.63960898899999996</v>
@@ -2212,7 +2217,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
-        <v>0.21068105925604311</v>
+        <v>0.22488822774398493</v>
       </c>
       <c r="F14">
         <v>0.159440161</v>
@@ -2225,7 +2230,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="1"/>
-        <v>0.53164631720137279</v>
+        <v>0.54595561439521068</v>
       </c>
       <c r="J14">
         <v>0.62727879200000003</v>
@@ -2301,7 +2306,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
-        <v>5.4992481052255057E-2</v>
+        <v>9.5981139922719824E-2</v>
       </c>
       <c r="F15">
         <v>0.68545622699999997</v>
@@ -2314,7 +2319,7 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" si="1"/>
-        <v>0.59748793706270309</v>
+        <v>0.61025532462348409</v>
       </c>
       <c r="J15">
         <v>0.62143581800000003</v>
@@ -2390,7 +2395,7 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
-        <v>6.2806362055221027E-2</v>
+        <v>0.10066203536186619</v>
       </c>
       <c r="F16">
         <v>0.299095638</v>
@@ -2403,7 +2408,7 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="1"/>
-        <v>0.33212315896859967</v>
+        <v>0.35457794491359862</v>
       </c>
       <c r="J16">
         <v>0.61644141799999996</v>
@@ -2479,7 +2484,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0.20953298491832723</v>
+        <v>0.22381304255419529</v>
       </c>
       <c r="F17">
         <v>1.2724831940000001</v>
@@ -2492,7 +2497,7 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" si="1"/>
-        <v>0.13474954467557768</v>
+        <v>0.18324073260643983</v>
       </c>
       <c r="J17">
         <v>0.63028568900000004</v>
@@ -2568,7 +2573,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="0"/>
-        <v>6.4585884793049622E-2</v>
+        <v>0.10178183906318046</v>
       </c>
       <c r="F18">
         <v>1.367313438</v>
@@ -2581,7 +2586,7 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" si="1"/>
-        <v>0.26113613004869141</v>
+        <v>0.28915705890169158</v>
       </c>
       <c r="J18">
         <v>0.62190721800000004</v>
@@ -2657,7 +2662,7 @@
       </c>
       <c r="E19" s="1">
         <f t="shared" si="0"/>
-        <v>0.1273239780956672</v>
+        <v>0.14966496466003001</v>
       </c>
       <c r="F19">
         <v>1.064157241</v>
@@ -2670,7 +2675,7 @@
       </c>
       <c r="I19" s="1">
         <f t="shared" si="1"/>
-        <v>0.11095176647416846</v>
+        <v>0.16652333403943029</v>
       </c>
       <c r="J19">
         <v>0.64641056200000002</v>
@@ -2746,7 +2751,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>6.9833533131594072E-2</v>
+        <v>0.10518996434177329</v>
       </c>
       <c r="F20">
         <v>1.9174821209999999</v>
@@ -2759,7 +2764,7 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" si="1"/>
-        <v>0.27773600284069538</v>
+        <v>0.30423184180784896</v>
       </c>
       <c r="J20">
         <v>0.62457086100000003</v>
@@ -2835,7 +2840,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0.30588429195300837</v>
+        <v>0.31583762649845148</v>
       </c>
       <c r="F21">
         <v>1.6455970470000001</v>
@@ -2848,7 +2853,7 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" si="1"/>
-        <v>0.2674037979778382</v>
+        <v>0.29482964143525625</v>
       </c>
       <c r="J21">
         <v>0.67833096800000003</v>
@@ -2924,7 +2929,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>0.55616883846059306</v>
+        <v>0.56170453365019879</v>
       </c>
       <c r="F22">
         <v>1.445542455</v>
@@ -2937,7 +2942,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" si="1"/>
-        <v>0.37552259282579992</v>
+        <v>0.39552110439075283</v>
       </c>
       <c r="J22">
         <v>0.656853087</v>
@@ -3013,7 +3018,7 @@
       </c>
       <c r="E23" s="1">
         <f t="shared" si="0"/>
-        <v>1.1979222065402254E-2</v>
+        <v>7.9572030323941778E-2</v>
       </c>
       <c r="F23">
         <v>0.90728684100000001</v>
@@ -3026,7 +3031,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="1"/>
-        <v>4.5245300672829593E-2</v>
+        <v>0.13216226212063723</v>
       </c>
       <c r="J23">
         <v>0.64625007999999995</v>
@@ -3102,7 +3107,7 @@
       </c>
       <c r="E24" s="1">
         <f t="shared" si="0"/>
-        <v>0.294044820594069</v>
+        <v>0.30438554953673524</v>
       </c>
       <c r="F24">
         <v>1.9607142820000001</v>
@@ -3115,7 +3120,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" si="1"/>
-        <v>0.61852040088179816</v>
+        <v>0.63086227704852471</v>
       </c>
       <c r="J24">
         <v>0.66231862799999996</v>
@@ -3191,7 +3196,7 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" si="0"/>
-        <v>9.8079971223957368E-2</v>
+        <v>0.12572941980250443</v>
       </c>
       <c r="F25">
         <v>1.113932506</v>
@@ -3204,7 +3209,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="1"/>
-        <v>1.0099848952886519</v>
+        <v>1.0175899051224411</v>
       </c>
       <c r="J25">
         <v>0.62905796199999997</v>
@@ -3280,7 +3285,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" si="0"/>
-        <v>0.27461003124209576</v>
+        <v>0.28565516887913456</v>
       </c>
       <c r="F26">
         <v>1.074293049</v>
@@ -3293,7 +3298,7 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" si="1"/>
-        <v>7.5707360872744073E-2</v>
+        <v>0.14543497098767258</v>
       </c>
       <c r="J26">
         <v>0.65236139000000004</v>
@@ -3352,6 +3357,17 @@
       <c r="AA26">
         <f t="shared" si="5"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32">
+        <v>7.8665152695345922E-2</v>
+      </c>
+      <c r="I32">
+        <v>0.12417619053534083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>